<commit_message>
Minden eddigi feladat leadása.
</commit_message>
<xml_diff>
--- a/QMHKMU_0416/Órai munka.xlsx
+++ b/QMHKMU_0416/Órai munka.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hallgató\Documents\GitHub\QMHKMU_OSGyak\QMHKMU_0416\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55FC1663-633B-45B6-9857-F9A7BE5807D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BEFF66-1043-43A3-BD33-0E8BA18724A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{223752D1-63A4-4AC6-B605-B3CF8D323848}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{223752D1-63A4-4AC6-B605-B3CF8D323848}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -352,12 +352,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -373,13 +369,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -716,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0E5F894-7800-464B-A485-1A8EC31E98A8}">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -730,12 +728,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
       <c r="F1" t="s">
         <v>10</v>
       </c>
@@ -744,24 +739,24 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="F2" s="1" t="s">
+      <c r="B2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="F2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="J2" s="1" t="s">
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="J2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -793,7 +788,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
@@ -828,16 +823,16 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4">
-        <v>3</v>
-      </c>
-      <c r="C5" s="4">
-        <v>2</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2">
         <v>2</v>
       </c>
       <c r="F5">
@@ -861,12 +856,12 @@
         <f t="shared" ref="L5:L8" si="3">D5-H5</f>
         <v>0</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6">
@@ -901,7 +896,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B7">
@@ -936,7 +931,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8">
@@ -988,7 +983,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F10">
@@ -1038,21 +1033,21 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="F15" s="1" t="s">
+      <c r="B15" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="F15" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="J15" s="1" t="s">
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="J15" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
@@ -1084,7 +1079,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B17">
@@ -1119,7 +1114,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B18">
@@ -1154,7 +1149,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B19">
@@ -1176,7 +1171,7 @@
         <v>1</v>
       </c>
       <c r="J19">
-        <f t="shared" ref="J18:J20" si="9">B19-F19</f>
+        <f t="shared" ref="J19:J20" si="9">B19-F19</f>
         <v>0</v>
       </c>
       <c r="K19">
@@ -1189,7 +1184,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B20">
@@ -1222,7 +1217,7 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="M20" s="4" t="s">
+      <c r="M20" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1247,7 +1242,7 @@
         <v>0</v>
       </c>
       <c r="H23">
-        <f t="shared" ref="G23:H23" si="10">H22-L20</f>
+        <f t="shared" ref="H23" si="10">H22-L20</f>
         <v>1</v>
       </c>
     </row>
@@ -1267,13 +1262,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="N2:P2"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="J15:L15"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="J2:L2"/>
-    <mergeCell ref="N2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -1284,8 +1279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F576D38-13DE-40F6-A27E-B00BC03706E0}">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1324,24 +1319,24 @@
       </c>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="C5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="G5" s="1" t="s">
+      <c r="C5" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="G5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
       <c r="K5" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
       <c r="R5" t="s">
         <v>23</v>
       </c>
@@ -1386,7 +1381,7 @@
       <c r="Q6" t="s">
         <v>4</v>
       </c>
-      <c r="R6" s="8" t="s">
+      <c r="R6" s="6" t="s">
         <v>24</v>
       </c>
       <c r="S6" t="s">
@@ -1439,7 +1434,7 @@
       <c r="Q7">
         <v>0</v>
       </c>
-      <c r="R7" s="8"/>
+      <c r="R7" s="6"/>
       <c r="S7">
         <f>K7-O7</f>
         <v>7</v>
@@ -1666,88 +1661,88 @@
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="G12" s="6">
+      <c r="G12" s="4">
         <f>SUM(G7:G11)</f>
         <v>7</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="4">
         <f t="shared" ref="H12:I12" si="4">SUM(H7:H11)</f>
         <v>2</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="4">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="O12" s="6">
+      <c r="O12" s="4">
         <f>SUM(O7:O11)</f>
         <v>8</v>
       </c>
-      <c r="P12" s="6">
+      <c r="P12" s="4">
         <f t="shared" ref="P12:Q12" si="5">SUM(P7:P11)</f>
         <v>2</v>
       </c>
-      <c r="Q12" s="6">
+      <c r="Q12" s="4">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="O13" s="9">
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="O13" s="7">
         <f>C2-O12</f>
         <v>2</v>
       </c>
-      <c r="P13" s="9">
+      <c r="P13" s="7">
         <f t="shared" ref="P13:Q13" si="6">D2-P12</f>
         <v>3</v>
       </c>
-      <c r="Q13" s="9">
+      <c r="Q13" s="7">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="12"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="10"/>
       <c r="E16" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="12"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="8" t="s">
+      <c r="B17" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="H17" s="15" t="s">
+      <c r="F17" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1755,25 +1750,25 @@
       <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="13">
-        <v>0</v>
-      </c>
-      <c r="C18" s="14">
-        <v>1</v>
-      </c>
-      <c r="D18" s="15">
-        <v>0</v>
-      </c>
-      <c r="E18" s="8" t="s">
+      <c r="B18" s="11">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="12">
+        <v>0</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="11">
         <v>7</v>
       </c>
-      <c r="G18" s="14">
-        <v>4</v>
-      </c>
-      <c r="H18" s="15">
+      <c r="G18">
+        <v>4</v>
+      </c>
+      <c r="H18" s="12">
         <v>3</v>
       </c>
     </row>
@@ -1781,22 +1776,22 @@
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="13">
-        <v>3</v>
-      </c>
-      <c r="C19" s="14">
-        <v>0</v>
-      </c>
-      <c r="D19" s="15">
-        <v>2</v>
-      </c>
-      <c r="F19" s="13">
+      <c r="B19" s="11">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" s="12">
+        <v>2</v>
+      </c>
+      <c r="F19" s="11">
         <v>6</v>
       </c>
-      <c r="G19" s="14">
-        <v>0</v>
-      </c>
-      <c r="H19" s="15">
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19" s="12">
         <v>0</v>
       </c>
     </row>
@@ -1804,25 +1799,25 @@
       <c r="A20" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="13">
-        <v>2</v>
-      </c>
-      <c r="C20" s="14">
-        <v>1</v>
-      </c>
-      <c r="D20" s="15">
-        <v>1</v>
-      </c>
-      <c r="F20" s="13">
-        <v>0</v>
-      </c>
-      <c r="G20" s="14">
-        <v>1</v>
-      </c>
-      <c r="H20" s="15">
-        <v>1</v>
-      </c>
-      <c r="I20" s="4" t="s">
+      <c r="B20" s="11">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="12">
+        <v>1</v>
+      </c>
+      <c r="F20" s="11">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" s="12">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1830,49 +1825,49 @@
       <c r="A21" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="13">
-        <v>0</v>
-      </c>
-      <c r="C21" s="14">
-        <v>0</v>
-      </c>
-      <c r="D21" s="15">
-        <v>2</v>
-      </c>
-      <c r="F21" s="16">
-        <v>4</v>
-      </c>
-      <c r="G21" s="17">
-        <v>3</v>
-      </c>
-      <c r="H21" s="18">
+      <c r="B21" s="11">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" s="12">
+        <v>2</v>
+      </c>
+      <c r="F21" s="13">
+        <v>4</v>
+      </c>
+      <c r="G21" s="14">
+        <v>3</v>
+      </c>
+      <c r="H21" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="13">
+      <c r="B22" s="11">
         <f>SUM(B18:B21)</f>
         <v>5</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="11">
         <f>SUM(C18:C21)</f>
         <v>2</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="16">
         <f>SUM(D18:D21)</f>
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="20">
+      <c r="B23" s="17">
         <f>C2-B22</f>
         <v>5</v>
       </c>
-      <c r="C23" s="20">
+      <c r="C23" s="17">
         <f t="shared" ref="C23:D23" si="7">D2-C22</f>
         <v>3</v>
       </c>
-      <c r="D23" s="20">
+      <c r="D23" s="17">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
@@ -1898,7 +1893,7 @@
       <c r="D26" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F26" t="s">
@@ -1924,7 +1919,7 @@
       <c r="D27">
         <v>0</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F27">
@@ -1998,15 +1993,15 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B31" s="6">
+      <c r="B31" s="4">
         <f>C2-B30</f>
         <v>7</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="4">
         <f t="shared" ref="C31:D31" si="9">D2-C30</f>
         <v>4</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="4">
         <f t="shared" si="9"/>
         <v>3</v>
       </c>

</xml_diff>